<commit_message>
Added metadata for each of the files
</commit_message>
<xml_diff>
--- a/191007_Deuterium_Transfer_Peak_Areas.xlsx
+++ b/191007_Deuterium_Transfer_Peak_Areas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Parker_research\GCMS_Stuff\191007\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017A9BEE-07BA-45DC-B87D-6B7C06262AC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2A6AAB-2FF9-4E77-B4C1-9E178F5A40FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4510" yWindow="7430" windowWidth="32550" windowHeight="15140" xr2:uid="{0C4FD04D-EEC1-4A1F-94F8-64C84F3860BB}"/>
+    <workbookView xWindow="19250" yWindow="170" windowWidth="18930" windowHeight="20190" xr2:uid="{0C4FD04D-EEC1-4A1F-94F8-64C84F3860BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="28">
   <si>
     <t>Species</t>
   </si>
@@ -93,9 +93,6 @@
     <t>#Type refers to deuterium labelled ants (L) vs unlabelled ants (U)</t>
   </si>
   <si>
-    <t>#Outlier: Beetle or ant crushed/Beetle or ant escaped from well/Ant not coated in any CHCs (Y), Beetle chomped (B), ant chomped (A), normal run (N)</t>
-  </si>
-  <si>
     <t>#GCMS data for experiment recorded on 191003</t>
   </si>
   <si>
@@ -112,6 +109,12 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>#Outlier: Beetle or ant crushed/Beetle or ant escaped from well/Ant not coated in any CHCs (Y), Beetle chomped (B), ant chomped (A), ant injured from the beginning(I) , normal run (N)</t>
   </si>
 </sst>
 </file>
@@ -466,14 +469,14 @@
   <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:L16"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
@@ -483,7 +486,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -524,10 +527,10 @@
         <v>11</v>
       </c>
       <c r="M4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" t="s">
         <v>22</v>
-      </c>
-      <c r="N4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -571,7 +574,7 @@
         <v>12</v>
       </c>
       <c r="N5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -615,7 +618,7 @@
         <v>12</v>
       </c>
       <c r="N6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -659,7 +662,7 @@
         <v>12</v>
       </c>
       <c r="N7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -703,7 +706,7 @@
         <v>12</v>
       </c>
       <c r="N8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -747,7 +750,7 @@
         <v>12</v>
       </c>
       <c r="N9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -791,7 +794,7 @@
         <v>12</v>
       </c>
       <c r="N10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -832,10 +835,10 @@
         <v>0.95</v>
       </c>
       <c r="M11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
@@ -876,10 +879,10 @@
         <v>1.59</v>
       </c>
       <c r="M12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
@@ -920,10 +923,10 @@
         <v>1.08</v>
       </c>
       <c r="M13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -964,10 +967,10 @@
         <v>0.97</v>
       </c>
       <c r="M14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
@@ -1008,10 +1011,10 @@
         <v>1.8</v>
       </c>
       <c r="M15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
@@ -1052,10 +1055,10 @@
         <v>1.39</v>
       </c>
       <c r="M16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
@@ -1096,10 +1099,10 @@
         <v>0.99</v>
       </c>
       <c r="M17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
@@ -1140,10 +1143,10 @@
         <v>1.56</v>
       </c>
       <c r="M18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
@@ -1184,10 +1187,10 @@
         <v>1.05</v>
       </c>
       <c r="M19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
@@ -1228,10 +1231,10 @@
         <v>0.99</v>
       </c>
       <c r="M20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
@@ -1272,10 +1275,10 @@
         <v>2.13</v>
       </c>
       <c r="M21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
@@ -1316,10 +1319,10 @@
         <v>0.7</v>
       </c>
       <c r="M22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
@@ -1363,7 +1366,7 @@
         <v>12</v>
       </c>
       <c r="N23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
@@ -1407,7 +1410,7 @@
         <v>12</v>
       </c>
       <c r="N24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
@@ -1451,7 +1454,7 @@
         <v>12</v>
       </c>
       <c r="N25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
@@ -1495,7 +1498,7 @@
         <v>12</v>
       </c>
       <c r="N26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
@@ -1539,7 +1542,7 @@
         <v>12</v>
       </c>
       <c r="N27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
@@ -1583,7 +1586,7 @@
         <v>12</v>
       </c>
       <c r="N28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
@@ -1624,10 +1627,10 @@
         <v>0.98</v>
       </c>
       <c r="M29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
@@ -1668,10 +1671,10 @@
         <v>1.63</v>
       </c>
       <c r="M30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
@@ -1712,10 +1715,10 @@
         <v>1.07</v>
       </c>
       <c r="M31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.35">
@@ -1756,10 +1759,10 @@
         <v>1.01</v>
       </c>
       <c r="M32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.35">
@@ -1800,10 +1803,10 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="M33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.35">
@@ -1844,10 +1847,10 @@
         <v>0.95</v>
       </c>
       <c r="M34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.35">
@@ -1891,7 +1894,7 @@
         <v>12</v>
       </c>
       <c r="N35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.35">
@@ -1935,7 +1938,7 @@
         <v>12</v>
       </c>
       <c r="N36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.35">
@@ -1979,7 +1982,7 @@
         <v>12</v>
       </c>
       <c r="N37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.35">
@@ -2023,7 +2026,7 @@
         <v>12</v>
       </c>
       <c r="N38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.35">
@@ -2067,7 +2070,7 @@
         <v>12</v>
       </c>
       <c r="N39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.35">
@@ -2111,7 +2114,7 @@
         <v>12</v>
       </c>
       <c r="N40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.35">
@@ -2155,7 +2158,7 @@
         <v>12</v>
       </c>
       <c r="N41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.35">
@@ -2199,7 +2202,7 @@
         <v>12</v>
       </c>
       <c r="N42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.35">
@@ -2243,7 +2246,7 @@
         <v>12</v>
       </c>
       <c r="N43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.35">
@@ -2287,7 +2290,7 @@
         <v>12</v>
       </c>
       <c r="N44" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.35">
@@ -2331,7 +2334,7 @@
         <v>12</v>
       </c>
       <c r="N45" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.35">
@@ -2375,7 +2378,7 @@
         <v>12</v>
       </c>
       <c r="N46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.35">
@@ -2416,10 +2419,10 @@
         <v>0.95</v>
       </c>
       <c r="M47" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N47" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.35">
@@ -2460,10 +2463,10 @@
         <v>2.27</v>
       </c>
       <c r="M48" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N48" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.35">
@@ -2504,10 +2507,10 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="M49" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N49" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.35">
@@ -2548,10 +2551,10 @@
         <v>0.97</v>
       </c>
       <c r="M50" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N50" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.35">
@@ -2592,10 +2595,10 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="M51" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N51" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.35">
@@ -2636,10 +2639,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="M52" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N52" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>